<commit_message>
Combined- Let role players add up to 6 account
</commit_message>
<xml_diff>
--- a/InteractiveWaterBudget/InteractiveWaterBudget-Mead.xlsx
+++ b/InteractiveWaterBudget/InteractiveWaterBudget-Mead.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverFutures\InteractiveWaterBudget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1A19A9-83E3-4E99-8417-96FA42440E4F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872C55A4-D3EE-4DB4-9CBB-96509D96FDB9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640" activeTab="2" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="198">
   <si>
     <t xml:space="preserve">    To Upper Basin</t>
   </si>
@@ -622,6 +622,12 @@
   <si>
     <t>Compensated Trades (+ sell to bank, - buy from bank)</t>
   </si>
+  <si>
+    <t>Lake Powell Release</t>
+  </si>
+  <si>
+    <t>Shared, Reserve</t>
+  </si>
 </sst>
 </file>
 
@@ -1031,14 +1037,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1053,6 +1053,12 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1064,6 +1070,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1071,9 +1080,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1094,154 +1100,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1472,6 +1330,154 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -21525,20 +21531,20 @@
       <c r="D3"/>
     </row>
     <row r="4" spans="1:12" ht="187.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="80" t="s">
         <v>142</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
-      <c r="K4" s="69"/>
-      <c r="L4" s="69"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="80"/>
+      <c r="K4" s="80"/>
+      <c r="L4" s="80"/>
     </row>
     <row r="5" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="15"/>
@@ -21554,218 +21560,218 @@
       <c r="L5" s="15"/>
     </row>
     <row r="6" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="73" t="s">
+      <c r="A6" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="74"/>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="74"/>
-      <c r="J6" s="74"/>
-      <c r="K6" s="74"/>
-      <c r="L6" s="75"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+      <c r="L6" s="73"/>
     </row>
     <row r="7" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="28">
         <v>1</v>
       </c>
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="74" t="s">
         <v>131</v>
       </c>
-      <c r="C7" s="70"/>
-      <c r="D7" s="70"/>
-      <c r="E7" s="70"/>
-      <c r="F7" s="70"/>
-      <c r="G7" s="70"/>
-      <c r="H7" s="70"/>
-      <c r="I7" s="70"/>
-      <c r="J7" s="70"/>
-      <c r="K7" s="70"/>
-      <c r="L7" s="71"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
+      <c r="L7" s="75"/>
     </row>
     <row r="8" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="28">
         <v>2</v>
       </c>
-      <c r="B8" s="70" t="s">
+      <c r="B8" s="74" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="70"/>
-      <c r="I8" s="70"/>
-      <c r="J8" s="70"/>
-      <c r="K8" s="70"/>
-      <c r="L8" s="71"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="74"/>
+      <c r="G8" s="74"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="74"/>
+      <c r="K8" s="74"/>
+      <c r="L8" s="75"/>
     </row>
     <row r="9" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="28">
         <v>3</v>
       </c>
-      <c r="B9" s="70" t="s">
+      <c r="B9" s="74" t="s">
         <v>132</v>
       </c>
-      <c r="C9" s="70"/>
-      <c r="D9" s="70"/>
-      <c r="E9" s="70"/>
-      <c r="F9" s="70"/>
-      <c r="G9" s="70"/>
-      <c r="H9" s="70"/>
-      <c r="I9" s="70"/>
-      <c r="J9" s="70"/>
-      <c r="K9" s="70"/>
-      <c r="L9" s="71"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="74"/>
+      <c r="L9" s="75"/>
     </row>
     <row r="10" spans="1:12" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="28">
         <v>4</v>
       </c>
-      <c r="B10" s="70" t="s">
+      <c r="B10" s="74" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="70"/>
-      <c r="D10" s="70"/>
-      <c r="E10" s="70"/>
-      <c r="F10" s="70"/>
-      <c r="G10" s="70"/>
-      <c r="H10" s="70"/>
-      <c r="I10" s="70"/>
-      <c r="J10" s="70"/>
-      <c r="K10" s="70"/>
-      <c r="L10" s="71"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
+      <c r="J10" s="74"/>
+      <c r="K10" s="74"/>
+      <c r="L10" s="75"/>
     </row>
     <row r="11" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="28">
         <v>5</v>
       </c>
-      <c r="B11" s="70" t="s">
+      <c r="B11" s="74" t="s">
         <v>133</v>
       </c>
-      <c r="C11" s="70"/>
-      <c r="D11" s="70"/>
-      <c r="E11" s="70"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="70"/>
-      <c r="H11" s="70"/>
-      <c r="I11" s="70"/>
-      <c r="J11" s="70"/>
-      <c r="K11" s="70"/>
-      <c r="L11" s="71"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="74"/>
+      <c r="J11" s="74"/>
+      <c r="K11" s="74"/>
+      <c r="L11" s="75"/>
     </row>
     <row r="12" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="28">
         <v>6</v>
       </c>
-      <c r="B12" s="70" t="s">
+      <c r="B12" s="74" t="s">
         <v>134</v>
       </c>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="70"/>
-      <c r="G12" s="70"/>
-      <c r="H12" s="70"/>
-      <c r="I12" s="70"/>
-      <c r="J12" s="70"/>
-      <c r="K12" s="70"/>
-      <c r="L12" s="71"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="74"/>
+      <c r="H12" s="74"/>
+      <c r="I12" s="74"/>
+      <c r="J12" s="74"/>
+      <c r="K12" s="74"/>
+      <c r="L12" s="75"/>
     </row>
     <row r="13" spans="1:12" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="28">
         <v>7</v>
       </c>
-      <c r="B13" s="70" t="s">
+      <c r="B13" s="74" t="s">
         <v>135</v>
       </c>
-      <c r="C13" s="70"/>
-      <c r="D13" s="70"/>
-      <c r="E13" s="70"/>
-      <c r="F13" s="70"/>
-      <c r="G13" s="70"/>
-      <c r="H13" s="70"/>
-      <c r="I13" s="70"/>
-      <c r="J13" s="70"/>
-      <c r="K13" s="70"/>
-      <c r="L13" s="71"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="74"/>
+      <c r="J13" s="74"/>
+      <c r="K13" s="74"/>
+      <c r="L13" s="75"/>
     </row>
     <row r="14" spans="1:12" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="28">
         <v>8</v>
       </c>
-      <c r="B14" s="70" t="s">
+      <c r="B14" s="74" t="s">
         <v>136</v>
       </c>
-      <c r="C14" s="70"/>
-      <c r="D14" s="70"/>
-      <c r="E14" s="70"/>
-      <c r="F14" s="70"/>
-      <c r="G14" s="70"/>
-      <c r="H14" s="70"/>
-      <c r="I14" s="70"/>
-      <c r="J14" s="70"/>
-      <c r="K14" s="70"/>
-      <c r="L14" s="71"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="74"/>
+      <c r="H14" s="74"/>
+      <c r="I14" s="74"/>
+      <c r="J14" s="74"/>
+      <c r="K14" s="74"/>
+      <c r="L14" s="75"/>
     </row>
     <row r="15" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="28">
         <v>9</v>
       </c>
-      <c r="B15" s="70" t="s">
+      <c r="B15" s="74" t="s">
         <v>137</v>
       </c>
-      <c r="C15" s="70"/>
-      <c r="D15" s="70"/>
-      <c r="E15" s="70"/>
-      <c r="F15" s="70"/>
-      <c r="G15" s="70"/>
-      <c r="H15" s="70"/>
-      <c r="I15" s="70"/>
-      <c r="J15" s="70"/>
-      <c r="K15" s="70"/>
-      <c r="L15" s="71"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="74"/>
+      <c r="I15" s="74"/>
+      <c r="J15" s="74"/>
+      <c r="K15" s="74"/>
+      <c r="L15" s="75"/>
     </row>
     <row r="16" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="28">
         <v>10</v>
       </c>
-      <c r="B16" s="70" t="s">
+      <c r="B16" s="74" t="s">
         <v>138</v>
       </c>
-      <c r="C16" s="70"/>
-      <c r="D16" s="70"/>
-      <c r="E16" s="70"/>
-      <c r="F16" s="70"/>
-      <c r="G16" s="70"/>
-      <c r="H16" s="70"/>
-      <c r="I16" s="70"/>
-      <c r="J16" s="70"/>
-      <c r="K16" s="70"/>
-      <c r="L16" s="71"/>
+      <c r="C16" s="74"/>
+      <c r="D16" s="74"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="74"/>
+      <c r="H16" s="74"/>
+      <c r="I16" s="74"/>
+      <c r="J16" s="74"/>
+      <c r="K16" s="74"/>
+      <c r="L16" s="75"/>
     </row>
     <row r="17" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="28">
         <v>11</v>
       </c>
-      <c r="B17" s="70" t="s">
+      <c r="B17" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="70"/>
-      <c r="D17" s="70"/>
-      <c r="E17" s="70"/>
-      <c r="F17" s="70"/>
-      <c r="G17" s="70"/>
-      <c r="H17" s="70"/>
-      <c r="I17" s="70"/>
-      <c r="J17" s="70"/>
-      <c r="K17" s="70"/>
-      <c r="L17" s="71"/>
+      <c r="C17" s="74"/>
+      <c r="D17" s="74"/>
+      <c r="E17" s="74"/>
+      <c r="F17" s="74"/>
+      <c r="G17" s="74"/>
+      <c r="H17" s="74"/>
+      <c r="I17" s="74"/>
+      <c r="J17" s="74"/>
+      <c r="K17" s="74"/>
+      <c r="L17" s="75"/>
     </row>
     <row r="18" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="28">
@@ -21891,23 +21897,28 @@
       </c>
     </row>
     <row r="32" spans="1:12" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="72" t="s">
+      <c r="A32" s="70" t="s">
         <v>141</v>
       </c>
-      <c r="B32" s="72"/>
-      <c r="C32" s="72"/>
-      <c r="D32" s="72"/>
-      <c r="E32" s="72"/>
-      <c r="F32" s="72"/>
-      <c r="G32" s="72"/>
-      <c r="H32" s="72"/>
-      <c r="I32" s="72"/>
-      <c r="J32" s="72"/>
-      <c r="K32" s="72"/>
-      <c r="L32" s="72"/>
+      <c r="B32" s="70"/>
+      <c r="C32" s="70"/>
+      <c r="D32" s="70"/>
+      <c r="E32" s="70"/>
+      <c r="F32" s="70"/>
+      <c r="G32" s="70"/>
+      <c r="H32" s="70"/>
+      <c r="I32" s="70"/>
+      <c r="J32" s="70"/>
+      <c r="K32" s="70"/>
+      <c r="L32" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="B9:L9"/>
+    <mergeCell ref="B11:L11"/>
+    <mergeCell ref="B12:L12"/>
+    <mergeCell ref="B13:L13"/>
     <mergeCell ref="A32:L32"/>
     <mergeCell ref="A6:L6"/>
     <mergeCell ref="B10:L10"/>
@@ -21919,11 +21930,6 @@
     <mergeCell ref="B18:L18"/>
     <mergeCell ref="B19:L19"/>
     <mergeCell ref="B14:L14"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="B9:L9"/>
-    <mergeCell ref="B11:L11"/>
-    <mergeCell ref="B12:L12"/>
-    <mergeCell ref="B13:L13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -21999,84 +22005,84 @@
         <v>53</v>
       </c>
       <c r="B5" s="52"/>
-      <c r="C5" s="82" t="s">
+      <c r="C5" s="83" t="s">
         <v>130</v>
       </c>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="82"/>
-      <c r="H5" s="82"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
         <v>157</v>
       </c>
       <c r="B6" s="52"/>
-      <c r="C6" s="82" t="s">
+      <c r="C6" s="83" t="s">
         <v>130</v>
       </c>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="82"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="83"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="83"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
         <v>158</v>
       </c>
       <c r="B7" s="52"/>
-      <c r="C7" s="82" t="s">
+      <c r="C7" s="83" t="s">
         <v>130</v>
       </c>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
+      <c r="D7" s="83"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="83"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
         <v>159</v>
       </c>
       <c r="B8" s="52"/>
-      <c r="C8" s="82" t="s">
+      <c r="C8" s="83" t="s">
         <v>130</v>
       </c>
-      <c r="D8" s="82"/>
-      <c r="E8" s="82"/>
-      <c r="F8" s="82"/>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
+      <c r="D8" s="83"/>
+      <c r="E8" s="83"/>
+      <c r="F8" s="83"/>
+      <c r="G8" s="83"/>
+      <c r="H8" s="83"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="16" t="s">
         <v>160</v>
       </c>
       <c r="B9" s="52"/>
-      <c r="C9" s="82" t="s">
+      <c r="C9" s="83" t="s">
         <v>192</v>
       </c>
-      <c r="D9" s="82"/>
-      <c r="E9" s="82"/>
-      <c r="F9" s="82"/>
-      <c r="G9" s="82"/>
-      <c r="H9" s="82"/>
+      <c r="D9" s="83"/>
+      <c r="E9" s="83"/>
+      <c r="F9" s="83"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="83"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B10" s="52"/>
-      <c r="C10" s="82" t="s">
+      <c r="C10" s="83" t="s">
         <v>130</v>
       </c>
-      <c r="D10" s="82"/>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="82"/>
+      <c r="D10" s="83"/>
+      <c r="E10" s="83"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="83"/>
+      <c r="H10" s="83"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="16"/>
@@ -22110,12 +22116,12 @@
       <c r="A17" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="80"/>
-      <c r="E17" s="81"/>
-      <c r="F17" s="81"/>
-      <c r="G17" s="81"/>
-      <c r="H17" s="81"/>
-      <c r="I17" s="81"/>
+      <c r="D17" s="81"/>
+      <c r="E17" s="82"/>
+      <c r="F17" s="82"/>
+      <c r="G17" s="82"/>
+      <c r="H17" s="82"/>
+      <c r="I17" s="82"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
@@ -24404,9 +24410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EABAA8-50C5-44CE-8E5C-AFA0657DFA46}">
   <dimension ref="A1:W75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -24470,84 +24474,84 @@
         <v>53</v>
       </c>
       <c r="B5" s="52"/>
-      <c r="C5" s="82" t="s">
+      <c r="C5" s="83" t="s">
         <v>130</v>
       </c>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="82"/>
-      <c r="H5" s="82"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
         <v>157</v>
       </c>
       <c r="B6" s="52"/>
-      <c r="C6" s="82" t="s">
+      <c r="C6" s="83" t="s">
         <v>130</v>
       </c>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="82"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="83"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="83"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
         <v>158</v>
       </c>
       <c r="B7" s="52"/>
-      <c r="C7" s="82" t="s">
+      <c r="C7" s="83" t="s">
         <v>130</v>
       </c>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
+      <c r="D7" s="83"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="83"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
         <v>159</v>
       </c>
       <c r="B8" s="52"/>
-      <c r="C8" s="82" t="s">
+      <c r="C8" s="83" t="s">
         <v>130</v>
       </c>
-      <c r="D8" s="82"/>
-      <c r="E8" s="82"/>
-      <c r="F8" s="82"/>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
+      <c r="D8" s="83"/>
+      <c r="E8" s="83"/>
+      <c r="F8" s="83"/>
+      <c r="G8" s="83"/>
+      <c r="H8" s="83"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="16" t="s">
-        <v>160</v>
+        <v>197</v>
       </c>
       <c r="B9" s="52"/>
-      <c r="C9" s="82" t="s">
+      <c r="C9" s="83" t="s">
         <v>192</v>
       </c>
-      <c r="D9" s="82"/>
-      <c r="E9" s="82"/>
-      <c r="F9" s="82"/>
-      <c r="G9" s="82"/>
-      <c r="H9" s="82"/>
+      <c r="D9" s="83"/>
+      <c r="E9" s="83"/>
+      <c r="F9" s="83"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="83"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B10" s="52"/>
-      <c r="C10" s="82" t="s">
+      <c r="C10" s="83" t="s">
         <v>130</v>
       </c>
-      <c r="D10" s="82"/>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="82"/>
+      <c r="D10" s="83"/>
+      <c r="E10" s="83"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="83"/>
+      <c r="H10" s="83"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="16"/>
@@ -24581,12 +24585,12 @@
       <c r="A17" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="80"/>
-      <c r="E17" s="81"/>
-      <c r="F17" s="81"/>
-      <c r="G17" s="81"/>
-      <c r="H17" s="81"/>
-      <c r="I17" s="81"/>
+      <c r="D17" s="81"/>
+      <c r="E17" s="82"/>
+      <c r="F17" s="82"/>
+      <c r="G17" s="82"/>
+      <c r="H17" s="82"/>
+      <c r="I17" s="82"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
@@ -24665,7 +24669,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>46</v>
+        <v>196</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="45">
@@ -25915,23 +25919,23 @@
       <c r="A55" s="31" t="s">
         <v>183</v>
       </c>
-      <c r="C55" s="83">
+      <c r="C55" s="69">
         <f t="shared" ref="C55:L55" si="19">IF(C$24&lt;&gt;"",C29+C41-C47,"")</f>
         <v>4.7720000000000002</v>
       </c>
-      <c r="D55" s="83">
+      <c r="D55" s="69">
         <f t="shared" si="19"/>
         <v>4.7720000000000011</v>
       </c>
-      <c r="E55" s="83">
+      <c r="E55" s="69">
         <f t="shared" si="19"/>
         <v>4.772000000000002</v>
       </c>
-      <c r="F55" s="83">
+      <c r="F55" s="69">
         <f t="shared" si="19"/>
         <v>4.7720000000000029</v>
       </c>
-      <c r="G55" s="83">
+      <c r="G55" s="69">
         <f t="shared" si="19"/>
         <v>4.7720000000000038</v>
       </c>
@@ -25960,23 +25964,23 @@
       <c r="A56" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C56" s="83">
+      <c r="C56" s="69">
         <f>IF(C$24&lt;&gt;"",C30+C42-C48,"")</f>
         <v>1.4490000000000001</v>
       </c>
-      <c r="D56" s="83">
-        <f t="shared" ref="C56:L56" si="20">IF(D$24&lt;&gt;"",D30+D42-D48,"")</f>
+      <c r="D56" s="69">
+        <f t="shared" ref="D56:L56" si="20">IF(D$24&lt;&gt;"",D30+D42-D48,"")</f>
         <v>1.4580000000000002</v>
       </c>
-      <c r="E56" s="83">
+      <c r="E56" s="69">
         <f t="shared" si="20"/>
         <v>1.4670000000000003</v>
       </c>
-      <c r="F56" s="83">
+      <c r="F56" s="69">
         <f t="shared" si="20"/>
         <v>1.4760000000000004</v>
       </c>
-      <c r="G56" s="83">
+      <c r="G56" s="69">
         <f t="shared" si="20"/>
         <v>1.4850000000000005</v>
       </c>
@@ -26160,7 +26164,7 @@
         <v>2.2879999999999998</v>
       </c>
       <c r="H60" s="43">
-        <f t="shared" ref="D60:L60" si="25">IF(H$24&lt;&gt;"",2.8-VLOOKUP(H$25,$O$60:$T$69,4)/1000000,"")</f>
+        <f t="shared" ref="H60:L60" si="25">IF(H$24&lt;&gt;"",2.8-VLOOKUP(H$25,$O$60:$T$69,4)/1000000,"")</f>
         <v>2.2879999999999998</v>
       </c>
       <c r="I60" s="43">
@@ -26237,7 +26241,7 @@
         <v>0.67200000000000004</v>
       </c>
       <c r="H61" s="43">
-        <f t="shared" ref="D61:L61" si="28">IF(H$24&lt;&gt;"",0.6,"")</f>
+        <f t="shared" ref="H61:L61" si="28">IF(H$24&lt;&gt;"",0.6,"")</f>
         <v>0.6</v>
       </c>
       <c r="I61" s="43">
@@ -26314,7 +26318,7 @@
         <v>1.44</v>
       </c>
       <c r="H62" s="43">
-        <f t="shared" ref="D62:L62" si="30">IF(H$24&lt;&gt;"",1.5-VLOOKUP(H$25,$O$60:$T$69,6),"")</f>
+        <f t="shared" ref="H62:L62" si="30">IF(H$24&lt;&gt;"",1.5-VLOOKUP(H$25,$O$60:$T$69,6),"")</f>
         <v>1.47</v>
       </c>
       <c r="I62" s="43">
@@ -27061,57 +27065,57 @@
     <mergeCell ref="C10:H10"/>
   </mergeCells>
   <conditionalFormatting sqref="C58:L62">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="11" operator="greaterThan">
       <formula>$C$52</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:L49">
-    <cfRule type="cellIs" dxfId="9" priority="10" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="39" priority="10" stopIfTrue="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:L49">
-    <cfRule type="cellIs" dxfId="8" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="9" stopIfTrue="1" operator="equal">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62:G62">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="8" operator="greaterThan">
       <formula>$C$56</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D62">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="7" operator="greaterThan">
       <formula>$D$56</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E62">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="6" operator="greaterThan">
       <formula>$E$56</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F62">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="5" operator="greaterThan">
       <formula>$F$56</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G62">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="4" operator="greaterThan">
       <formula>$G$56</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:G59">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="3" operator="greaterThan">
       <formula>$C$53</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:G60">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="2" operator="greaterThan">
       <formula>$C$54</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61:G61">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="1" operator="greaterThan">
       <formula>$C$55</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27189,84 +27193,84 @@
         <v>53</v>
       </c>
       <c r="B5" s="34"/>
-      <c r="C5" s="82" t="s">
+      <c r="C5" s="83" t="s">
         <v>130</v>
       </c>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="82"/>
-      <c r="H5" s="82"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
         <v>157</v>
       </c>
       <c r="B6" s="34"/>
-      <c r="C6" s="82" t="s">
+      <c r="C6" s="83" t="s">
         <v>130</v>
       </c>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="82"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="83"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="83"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
         <v>158</v>
       </c>
       <c r="B7" s="34"/>
-      <c r="C7" s="82" t="s">
+      <c r="C7" s="83" t="s">
         <v>130</v>
       </c>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
+      <c r="D7" s="83"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="83"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
         <v>159</v>
       </c>
       <c r="B8" s="34"/>
-      <c r="C8" s="82" t="s">
+      <c r="C8" s="83" t="s">
         <v>130</v>
       </c>
-      <c r="D8" s="82"/>
-      <c r="E8" s="82"/>
-      <c r="F8" s="82"/>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
+      <c r="D8" s="83"/>
+      <c r="E8" s="83"/>
+      <c r="F8" s="83"/>
+      <c r="G8" s="83"/>
+      <c r="H8" s="83"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="16" t="s">
         <v>160</v>
       </c>
       <c r="B9" s="52"/>
-      <c r="C9" s="82" t="s">
+      <c r="C9" s="83" t="s">
         <v>192</v>
       </c>
-      <c r="D9" s="82"/>
-      <c r="E9" s="82"/>
-      <c r="F9" s="82"/>
-      <c r="G9" s="82"/>
-      <c r="H9" s="82"/>
+      <c r="D9" s="83"/>
+      <c r="E9" s="83"/>
+      <c r="F9" s="83"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="83"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B10" s="52"/>
-      <c r="C10" s="82" t="s">
+      <c r="C10" s="83" t="s">
         <v>130</v>
       </c>
-      <c r="D10" s="82"/>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="82"/>
+      <c r="D10" s="83"/>
+      <c r="E10" s="83"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="83"/>
+      <c r="H10" s="83"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="16"/>
@@ -27300,12 +27304,12 @@
       <c r="A17" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="80"/>
-      <c r="E17" s="81"/>
-      <c r="F17" s="81"/>
-      <c r="G17" s="81"/>
-      <c r="H17" s="81"/>
-      <c r="I17" s="81"/>
+      <c r="D17" s="81"/>
+      <c r="E17" s="82"/>
+      <c r="F17" s="82"/>
+      <c r="G17" s="82"/>
+      <c r="H17" s="82"/>
+      <c r="I17" s="82"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
@@ -29754,37 +29758,37 @@
     <mergeCell ref="C10:H10"/>
   </mergeCells>
   <conditionalFormatting sqref="C58:L62">
-    <cfRule type="cellIs" dxfId="17" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="7" operator="greaterThan">
       <formula>$C$52</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:L49">
-    <cfRule type="cellIs" dxfId="16" priority="6" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="28" priority="6" stopIfTrue="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:L49">
-    <cfRule type="cellIs" dxfId="15" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="5" stopIfTrue="1" operator="equal">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:L59">
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="4" operator="greaterThan">
       <formula>$C$53</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:L60">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="greaterThan">
       <formula>$C$54</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61:L61">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="greaterThan">
       <formula>$C$55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62:L62">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="greaterThan">
       <formula>$C$56</formula>
     </cfRule>
   </conditionalFormatting>
@@ -59855,48 +59859,48 @@
         <v>53</v>
       </c>
       <c r="B5" s="49"/>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="82"/>
-      <c r="H5" s="82"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
         <v>41</v>
       </c>
       <c r="B6" s="49"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="82"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="83"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="83"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="49"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="83"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="83"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="49"/>
-      <c r="C8" s="82"/>
-      <c r="D8" s="82"/>
-      <c r="E8" s="82"/>
-      <c r="F8" s="82"/>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="83"/>
+      <c r="E8" s="83"/>
+      <c r="F8" s="83"/>
+      <c r="G8" s="83"/>
+      <c r="H8" s="83"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="16"/>
@@ -61603,117 +61607,117 @@
     <mergeCell ref="C8:H8"/>
   </mergeCells>
   <conditionalFormatting sqref="H49:L49">
-    <cfRule type="cellIs" dxfId="40" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="greaterThan">
       <formula>$C$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49">
-    <cfRule type="cellIs" dxfId="39" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="22" operator="greaterThan">
       <formula>$H$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I49">
-    <cfRule type="cellIs" dxfId="38" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="21" operator="greaterThan">
       <formula>$I$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J49">
-    <cfRule type="cellIs" dxfId="37" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="greaterThan">
       <formula>$J$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K49">
-    <cfRule type="cellIs" dxfId="36" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="19" operator="greaterThan">
       <formula>$K$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L49">
-    <cfRule type="cellIs" dxfId="35" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="greaterThan">
       <formula>$L$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H50:L50">
-    <cfRule type="cellIs" dxfId="34" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="greaterThan">
       <formula>$D$46</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H50">
-    <cfRule type="cellIs" dxfId="33" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="greaterThan">
       <formula>$H$46</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I50">
-    <cfRule type="cellIs" dxfId="32" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="greaterThan">
       <formula>$I$46</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J50">
-    <cfRule type="cellIs" dxfId="31" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="greaterThan">
       <formula>$J$46</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K50">
-    <cfRule type="cellIs" dxfId="30" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="greaterThan">
       <formula>$K$46</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L50">
-    <cfRule type="cellIs" dxfId="29" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="greaterThan">
       <formula>$L$46</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52">
-    <cfRule type="cellIs" dxfId="28" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="greaterThan">
       <formula>$C$47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52">
-    <cfRule type="cellIs" dxfId="27" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="greaterThan">
       <formula>$D$47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="cellIs" dxfId="26" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThan">
       <formula>$E$47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F52">
-    <cfRule type="cellIs" dxfId="25" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
       <formula>$F$47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G52">
-    <cfRule type="cellIs" dxfId="24" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
       <formula>$G$47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52">
-    <cfRule type="cellIs" dxfId="23" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
       <formula>$H$47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I52">
-    <cfRule type="cellIs" dxfId="22" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
       <formula>$I$47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J52">
-    <cfRule type="cellIs" dxfId="21" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>$J$47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K52">
-    <cfRule type="cellIs" dxfId="20" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>$K$47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L52">
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>$L$47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:G49">
-    <cfRule type="cellIs" dxfId="18" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>$C$45</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>